<commit_message>
Firm cambio de verciones
</commit_message>
<xml_diff>
--- a/Firmware/v0.3 Stable - Hard 0.0 to v0.2/LCD Layout - Firm v03.xlsx
+++ b/Firmware/v0.3 Stable - Hard 0.0 to v0.2/LCD Layout - Firm v03.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="73">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="699" uniqueCount="67">
   <si>
     <t>01</t>
   </si>
@@ -195,6 +195,9 @@
     <t>F</t>
   </si>
   <si>
+    <t>w</t>
+  </si>
+  <si>
     <t>S</t>
   </si>
   <si>
@@ -204,37 +207,16 @@
     <t>A</t>
   </si>
   <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
     <t>k</t>
   </si>
   <si>
-    <t>f</t>
-  </si>
-  <si>
-    <t>g</t>
-  </si>
-  <si>
-    <t>B</t>
-  </si>
-  <si>
     <t>=</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>&amp;</t>
-  </si>
-  <si>
-    <t>/</t>
-  </si>
-  <si>
-    <t>Y</t>
-  </si>
-  <si>
-    <t>j</t>
-  </si>
-  <si>
-    <t>7</t>
   </si>
 </sst>
 </file>
@@ -627,10 +609,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr codeName="Hoja1"/>
-  <dimension ref="A1:AF71"/>
+  <dimension ref="A1:AF65"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A52" workbookViewId="0">
-      <selection activeCell="W71" sqref="W71"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="W63" sqref="W63"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -719,135 +701,138 @@
       <c r="A2" s="2" t="s">
         <v>53</v>
       </c>
+      <c r="B2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>29</v>
+      </c>
       <c r="E2" s="1" t="s">
-        <v>61</v>
+        <v>22</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>45</v>
+        <v>30</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="H2" s="1" t="s">
-        <v>52</v>
+        <v>31</v>
       </c>
       <c r="I2" s="1" t="s">
         <v>32</v>
       </c>
       <c r="J2" s="1" t="s">
-        <v>24</v>
+        <v>33</v>
       </c>
       <c r="K2" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="N2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="M2" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>39</v>
-      </c>
       <c r="O2" s="1" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="P2" s="1" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="Q2" s="1" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="S2" s="1" t="s">
-        <v>42</v>
+        <v>37</v>
       </c>
     </row>
     <row r="3" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
+      <c r="B3" s="1" t="s">
+        <v>38</v>
+      </c>
       <c r="C3" s="1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>31</v>
+        <v>20</v>
       </c>
       <c r="F3" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="H3" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="N3" s="1" t="s">
         <v>44</v>
       </c>
-      <c r="G3" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="H3" s="1" t="s">
+      <c r="O3" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="J3" s="1" t="s">
-        <v>68</v>
-      </c>
-      <c r="L3" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="M3" s="1" t="s">
+      <c r="P3" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="N3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="O3" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="P3" s="1" t="s">
-        <v>45</v>
-      </c>
       <c r="Q3" s="1" t="s">
-        <v>35</v>
+        <v>26</v>
       </c>
       <c r="R3" s="1" t="s">
         <v>26</v>
       </c>
       <c r="S3" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="T3" s="1" t="s">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="U3" s="1" t="s">
-        <v>45</v>
+        <v>63</v>
       </c>
     </row>
     <row r="4" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="I4" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="C4" s="1" t="s">
+      <c r="J4" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="K4" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="E4" s="1" t="s">
+      <c r="L4" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="G4" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I4" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J4" s="1" t="s">
-        <v>19</v>
-      </c>
       <c r="M4" s="1" t="s">
-        <v>48</v>
+        <v>59</v>
       </c>
       <c r="N4" s="1" t="s">
         <v>23</v>
@@ -856,7 +841,10 @@
         <v>45</v>
       </c>
       <c r="P4" s="1" t="s">
-        <v>33</v>
+        <v>25</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>27</v>
       </c>
       <c r="R4" s="1" t="s">
         <v>47</v>
@@ -876,64 +864,58 @@
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>22</v>
+        <v>30</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>54</v>
+        <v>19</v>
       </c>
       <c r="F5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="I5" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="J5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="N5" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="O5" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="Q5" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="H5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="I5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="J5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="K5" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="L5" s="1" t="s">
+      <c r="R5" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="M5" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="N5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O5" s="1" t="s">
-        <v>69</v>
-      </c>
-      <c r="P5" s="1" t="s">
-        <v>62</v>
-      </c>
-      <c r="Q5" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="R5" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="S5" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="T5" s="1" t="s">
-        <v>71</v>
-      </c>
       <c r="U5" s="1" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
     </row>
     <row r="7" spans="1:32" s="3" customFormat="1" x14ac:dyDescent="0.25">
@@ -1055,7 +1037,7 @@
       <c r="Q8" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="R8" s="5" t="s">
+      <c r="R8" s="1" t="s">
         <v>20</v>
       </c>
       <c r="S8" s="1" t="s">
@@ -1524,7 +1506,7 @@
       </c>
       <c r="B22" s="5"/>
       <c r="C22" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D22" s="1" t="s">
         <v>23</v>
@@ -2040,7 +2022,7 @@
         <v>55</v>
       </c>
       <c r="L39" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="M39" s="1" t="s">
         <v>23</v>
@@ -2313,44 +2295,25 @@
       <c r="A51" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="C51" s="5"/>
-      <c r="D51" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="E51" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="F51" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="G51" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="H51" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I51" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="M51" s="5"/>
-      <c r="N51" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="O51" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="P51" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="Q51" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="R51" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="S51" s="1" t="s">
-        <v>64</v>
-      </c>
+      <c r="B51" s="6"/>
+      <c r="C51" s="6"/>
+      <c r="D51" s="6"/>
+      <c r="E51" s="6"/>
+      <c r="F51" s="6"/>
+      <c r="G51" s="6"/>
+      <c r="H51" s="6"/>
+      <c r="I51" s="6"/>
+      <c r="J51" s="6"/>
+      <c r="K51" s="6"/>
+      <c r="L51" s="6"/>
+      <c r="M51" s="6"/>
+      <c r="N51" s="6"/>
+      <c r="O51" s="6"/>
+      <c r="P51" s="6"/>
+      <c r="Q51" s="6"/>
+      <c r="R51" s="6"/>
+      <c r="S51" s="6"/>
+      <c r="T51" s="6"/>
     </row>
     <row r="52" spans="1:21" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
@@ -2543,7 +2506,7 @@
         <v>51</v>
       </c>
       <c r="P56" s="1" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="Q56" s="1" t="s">
         <v>56</v>
@@ -2670,7 +2633,7 @@
         <v>2</v>
       </c>
       <c r="B59" s="6" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C59" s="1" t="s">
         <v>52</v>
@@ -2705,7 +2668,7 @@
       </c>
       <c r="O59" s="5"/>
       <c r="P59" s="6" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="Q59" s="1" t="s">
         <v>54</v>
@@ -2854,19 +2817,16 @@
         <v>37</v>
       </c>
       <c r="O63" s="1" t="s">
-        <v>41</v>
+        <v>9</v>
       </c>
       <c r="P63" s="1" t="s">
-        <v>19</v>
+        <v>66</v>
       </c>
       <c r="Q63" s="1" t="s">
-        <v>66</v>
+        <v>36</v>
       </c>
       <c r="R63" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="S63" s="1" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
     </row>
     <row r="64" spans="1:21" x14ac:dyDescent="0.25">
@@ -2955,7 +2915,7 @@
       </c>
       <c r="P65" s="5"/>
       <c r="Q65" s="6" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="R65" s="1" t="s">
         <v>44</v>
@@ -2968,259 +2928,6 @@
       </c>
       <c r="U65" s="1" t="s">
         <v>44</v>
-      </c>
-    </row>
-    <row r="67" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A67" s="4"/>
-      <c r="B67" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="C67" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D67" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E67" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="F67" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="G67" s="2" t="s">
-        <v>4</v>
-      </c>
-      <c r="H67" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="I67" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="J67" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="K67" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="L67" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="M67" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="N67" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="O67" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="P67" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q67" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="R67" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="S67" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="T67" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="U67" s="2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="68" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A68" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="B68" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="D68" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="E68" s="1" t="s">
-        <v>63</v>
-      </c>
-      <c r="F68" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>64</v>
-      </c>
-      <c r="I68" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="J68" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K68" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="L68" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P68" s="5"/>
-      <c r="Q68" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="R68" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="S68" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="T68" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="U68" s="1" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="69" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A69" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="E69" s="6" t="s">
-        <v>65</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="G69" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="H69" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="J69" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="K69" s="6" t="s">
-        <v>32</v>
-      </c>
-      <c r="L69" s="6" t="s">
-        <v>64</v>
-      </c>
-      <c r="M69" s="6" t="s">
-        <v>22</v>
-      </c>
-      <c r="N69" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="O69" s="6" t="s">
-        <v>27</v>
-      </c>
-      <c r="P69" s="5"/>
-      <c r="Q69" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R69" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="S69" s="6" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="70" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A70" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="H70" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="I70" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="J70" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="K70" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="L70" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="M70" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="N70" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="O70" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P70" s="5"/>
-      <c r="Q70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="R70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="S70" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="T70" s="6"/>
-    </row>
-    <row r="71" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A71" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="B71" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C71" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="D71" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="E71" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F71" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="G71" s="1" t="s">
-        <v>45</v>
-      </c>
-      <c r="I71" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="J71" s="6" t="s">
-        <v>20</v>
-      </c>
-      <c r="K71" s="6" t="s">
-        <v>42</v>
-      </c>
-      <c r="L71" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="M71" s="6" t="s">
-        <v>43</v>
-      </c>
-      <c r="P71" s="5"/>
-      <c r="Q71" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="R71" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="S71" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="T71" s="6" t="s">
-        <v>26</v>
       </c>
     </row>
   </sheetData>

</xml_diff>